<commit_message>
Update LED Array V1.3 manufacturing files
</commit_message>
<xml_diff>
--- a/Electronic Design/Core64 LA v1.3 KiCAD 6/C64_LA_V1.3 Manufacturing by ELECROW/Core64 LA v1.3_BOM_sub-kit_Assembly.xlsx
+++ b/Electronic Design/Core64 LA v1.3 KiCAD 6/C64_LA_V1.3 Manufacturing by ELECROW/Core64 LA v1.3_BOM_sub-kit_Assembly.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewgeppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/Core64 LA v1.3 KiCAD 6/C64_LA_V1.3 Manufacturing by ELECROW/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/Core64 LA v1.3 KiCAD 6/C64_LA_V1.3 Manufacturing by ELECROW/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798FFAB2-E0D6-3843-A396-80A39258DD66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316BDEE2-FFDD-1143-B95B-49251AB81336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="61">
   <si>
     <t>Description</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>Bag, Antistatic, Closure, Clear or Blue, 5x8 inch</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/olimex-ltd/KAPTON-TAPE10MM/19204468</t>
   </si>
 </sst>
 </file>
@@ -743,7 +746,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -953,7 +956,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="2" customFormat="1" ht="17">
+    <row r="6" spans="1:12" s="2" customFormat="1" ht="45">
       <c r="A6" s="11" t="s">
         <v>40</v>
       </c>
@@ -981,8 +984,8 @@
       <c r="I6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="9" t="s">
-        <v>12</v>
+      <c r="J6" s="20" t="s">
+        <v>60</v>
       </c>
       <c r="K6" s="9" t="s">
         <v>12</v>
@@ -1270,6 +1273,7 @@
     <hyperlink ref="J12" r:id="rId8" xr:uid="{7B075D44-5647-444E-A258-BE60F2768E83}"/>
     <hyperlink ref="J13" r:id="rId9" xr:uid="{52F4E0F8-3D01-8647-9CA3-24374433F64D}"/>
     <hyperlink ref="K13" r:id="rId10" xr:uid="{C4FFCD72-791C-D248-B0E3-BC7F3C3B7147}"/>
+    <hyperlink ref="J6" r:id="rId11" xr:uid="{13E0BA90-E061-8C44-8DF9-A60FD89405E5}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>

</xml_diff>